<commit_message>
physics fix for 2tLotM
</commit_message>
<xml_diff>
--- a/Physics model templates/physics-table.xlsx
+++ b/Physics model templates/physics-table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
   <si>
     <t xml:space="preserve">defender cluts</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">orb allegiance</t>
   </si>
   <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
     <t xml:space="preserve">far side</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">2 and 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civilian S’pht non-alien, friendly</t>
   </si>
   <si>
     <t xml:space="preserve">eat spht</t>
@@ -442,10 +448,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,7 +465,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.5"/>
@@ -507,41 +513,44 @@
       <c r="M2" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="N2" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,7 +558,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" s="5"/>
       <c r="J4" s="6"/>
@@ -559,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5"/>
       <c r="J5" s="6"/>
@@ -569,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5"/>
       <c r="J6" s="6"/>
@@ -579,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="5"/>
       <c r="J7" s="6"/>
@@ -589,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="6"/>
@@ -599,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="6"/>
@@ -609,7 +618,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H10" s="5"/>
       <c r="J10" s="6"/>
@@ -619,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H11" s="5"/>
       <c r="J11" s="6"/>
@@ -629,7 +638,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H12" s="5"/>
       <c r="J12" s="6"/>
@@ -639,7 +648,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H13" s="5"/>
       <c r="J13" s="6"/>
@@ -649,7 +658,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H14" s="5"/>
       <c r="J14" s="6"/>
@@ -659,22 +668,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H15" s="5"/>
       <c r="J15" s="6"/>
@@ -684,22 +693,22 @@
         <v>13</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16" s="5"/>
       <c r="J16" s="6"/>
@@ -709,22 +718,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H17" s="5"/>
       <c r="J17" s="6"/>
@@ -734,22 +743,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" s="5"/>
       <c r="J18" s="6"/>
@@ -759,22 +768,22 @@
         <v>16</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H19" s="5"/>
       <c r="J19" s="6"/>
@@ -784,7 +793,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="5"/>
       <c r="J20" s="6"/>
@@ -794,7 +803,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H21" s="5"/>
       <c r="J21" s="6"/>
@@ -804,7 +813,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H22" s="5"/>
       <c r="J22" s="6"/>
@@ -814,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H23" s="5"/>
       <c r="J23" s="6"/>
@@ -824,28 +833,28 @@
         <v>21</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,28 +862,28 @@
         <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,28 +891,28 @@
         <v>23</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,25 +920,28 @@
         <v>24</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,25 +949,28 @@
         <v>25</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>54</v>
+      <c r="N28" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,25 +978,28 @@
         <v>26</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,13 +1007,13 @@
         <v>27</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -1004,13 +1022,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J31" s="6"/>
     </row>
@@ -1019,13 +1037,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G32" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="H32" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -1034,7 +1052,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H33" s="5"/>
       <c r="J33" s="6"/>
@@ -1044,12 +1062,12 @@
         <v>31</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H34" s="5"/>
       <c r="J34" s="6"/>
       <c r="K34" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L34" s="0" t="n">
         <v>7</v>
@@ -1060,12 +1078,12 @@
         <v>32</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H35" s="5"/>
       <c r="J35" s="6"/>
       <c r="K35" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L35" s="0" t="n">
         <v>7</v>
@@ -1076,12 +1094,12 @@
         <v>33</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H36" s="5"/>
       <c r="J36" s="6"/>
       <c r="K36" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L36" s="0" t="n">
         <v>7</v>
@@ -1092,12 +1110,12 @@
         <v>34</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H37" s="5"/>
       <c r="J37" s="6"/>
       <c r="K37" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L37" s="0" t="n">
         <v>7</v>
@@ -1108,12 +1126,12 @@
         <v>35</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H38" s="5"/>
       <c r="J38" s="6"/>
       <c r="K38" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L38" s="0" t="n">
         <v>7</v>
@@ -1124,18 +1142,18 @@
         <v>36</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H39" s="5"/>
       <c r="J39" s="6"/>
       <c r="K39" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L39" s="0" t="n">
         <v>7</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,12 +1161,12 @@
         <v>37</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H40" s="5"/>
       <c r="J40" s="6"/>
       <c r="K40" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L40" s="0" t="n">
         <v>7</v>
@@ -1159,12 +1177,12 @@
         <v>38</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H41" s="5"/>
       <c r="J41" s="6"/>
       <c r="K41" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L41" s="0" t="n">
         <v>7</v>
@@ -1175,12 +1193,12 @@
         <v>39</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H42" s="5"/>
       <c r="J42" s="6"/>
       <c r="K42" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L42" s="0" t="n">
         <v>7</v>
@@ -1191,7 +1209,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H43" s="5"/>
       <c r="J43" s="6"/>
@@ -1201,7 +1219,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H44" s="5"/>
       <c r="J44" s="6"/>
@@ -1211,7 +1229,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H45" s="5"/>
       <c r="J45" s="6"/>
@@ -1221,7 +1239,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H46" s="5"/>
       <c r="J46" s="6"/>
@@ -1231,7 +1249,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H47" s="5"/>
       <c r="J47" s="6"/>
@@ -1241,7 +1259,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H48" s="5"/>
       <c r="J48" s="6"/>
@@ -1251,7 +1269,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H49" s="5"/>
       <c r="J49" s="6"/>
@@ -1261,7 +1279,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H50" s="5"/>
       <c r="J50" s="6"/>
@@ -1271,7 +1289,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H51" s="5"/>
       <c r="J51" s="6"/>
@@ -1281,7 +1299,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H52" s="5"/>
       <c r="J52" s="6"/>
@@ -1291,7 +1309,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H53" s="5"/>
       <c r="J53" s="6"/>
@@ -1301,7 +1319,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H54" s="5"/>
       <c r="J54" s="6"/>

</xml_diff>

<commit_message>
skitter physics & table update
</commit_message>
<xml_diff>
--- a/Physics model templates/physics-table.xlsx
+++ b/Physics model templates/physics-table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="90">
   <si>
     <t xml:space="preserve">defender cluts</t>
   </si>
@@ -169,6 +169,12 @@
     <t xml:space="preserve">2 and 6</t>
   </si>
   <si>
+    <t xml:space="preserve">Fighters use CLUTs 4,5,6,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troopers use CLUTs 4,5</t>
+  </si>
+  <si>
     <t xml:space="preserve">sleeping gods</t>
   </si>
   <si>
@@ -218,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">vs player and pfhor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troopers use CLUTs 2,3</t>
   </si>
   <si>
     <t xml:space="preserve">incredible</t>
@@ -448,10 +457,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O14" activeCellId="0" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -469,7 +478,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,13 +867,19 @@
       <c r="J24" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="O24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>42</v>
@@ -884,6 +901,12 @@
       </c>
       <c r="J25" s="6" t="s">
         <v>48</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +914,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>42</v>
@@ -913,6 +936,12 @@
       </c>
       <c r="J26" s="6" t="s">
         <v>48</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,16 +949,16 @@
         <v>24</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>46</v>
@@ -938,10 +967,16 @@
         <v>47</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,16 +984,16 @@
         <v>25</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>46</v>
@@ -967,10 +1002,16 @@
         <v>47</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,16 +1019,16 @@
         <v>26</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>46</v>
@@ -996,10 +1037,16 @@
         <v>47</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,52 +1054,70 @@
         <v>27</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J30" s="6"/>
+      <c r="O30" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>28</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J31" s="6"/>
+      <c r="O31" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P31" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="6"/>
+      <c r="O32" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P32" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H33" s="5"/>
       <c r="J33" s="6"/>
@@ -1062,15 +1127,18 @@
         <v>31</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H34" s="5"/>
       <c r="J34" s="6"/>
       <c r="K34" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L34" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,15 +1146,18 @@
         <v>32</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H35" s="5"/>
       <c r="J35" s="6"/>
       <c r="K35" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L35" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="O35" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,15 +1165,18 @@
         <v>33</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H36" s="5"/>
       <c r="J36" s="6"/>
       <c r="K36" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L36" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,7 +1184,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H37" s="5"/>
       <c r="J37" s="6"/>
@@ -1120,13 +1194,16 @@
       <c r="L37" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="O37" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>35</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H38" s="5"/>
       <c r="J38" s="6"/>
@@ -1136,13 +1213,16 @@
       <c r="L38" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="O38" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>36</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H39" s="5"/>
       <c r="J39" s="6"/>
@@ -1153,7 +1233,10 @@
         <v>7</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,7 +1244,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H40" s="5"/>
       <c r="J40" s="6"/>
@@ -1171,13 +1254,16 @@
       <c r="L40" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="O40" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>38</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H41" s="5"/>
       <c r="J41" s="6"/>
@@ -1187,13 +1273,16 @@
       <c r="L41" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="O41" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>39</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H42" s="5"/>
       <c r="J42" s="6"/>
@@ -1203,13 +1292,16 @@
       <c r="L42" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="O42" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>40</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H43" s="5"/>
       <c r="J43" s="6"/>
@@ -1219,7 +1311,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H44" s="5"/>
       <c r="J44" s="6"/>
@@ -1229,7 +1321,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H45" s="5"/>
       <c r="J45" s="6"/>
@@ -1239,7 +1331,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H46" s="5"/>
       <c r="J46" s="6"/>
@@ -1249,7 +1341,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H47" s="5"/>
       <c r="J47" s="6"/>
@@ -1259,7 +1351,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H48" s="5"/>
       <c r="J48" s="6"/>
@@ -1269,7 +1361,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H49" s="5"/>
       <c r="J49" s="6"/>
@@ -1279,7 +1371,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H50" s="5"/>
       <c r="J50" s="6"/>
@@ -1289,7 +1381,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H51" s="5"/>
       <c r="J51" s="6"/>
@@ -1299,7 +1391,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H52" s="5"/>
       <c r="J52" s="6"/>
@@ -1309,7 +1401,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H53" s="5"/>
       <c r="J53" s="6"/>
@@ -1319,7 +1411,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H54" s="5"/>
       <c r="J54" s="6"/>

</xml_diff>